<commit_message>
New version of the checklist
</commit_message>
<xml_diff>
--- a/Checklists/DetailedChecklists.xlsx
+++ b/Checklists/DetailedChecklists.xlsx
@@ -836,15 +836,15 @@
     <t>Verify the selected dropdown value is displayed accordingly when user try to navigate to previous screen and navigate back to company details screen.</t>
   </si>
   <si>
-    <t>Dropdown value should be delected</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Click on the "Where’s your company registered?" dropdown and select "Sweden" from the dropdown.
 2. click on 'Back' and then 'Next Step'
 </t>
   </si>
   <si>
     <t>The selected dropdown  value should be displayed.</t>
+  </si>
+  <si>
+    <t>Dropdown value should be selected</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1653,7 +1653,7 @@
         <v>253</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>68</v>
@@ -1662,13 +1662,13 @@
         <v>124</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>63</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>